<commit_message>
Updated Doddegrasweg 12 te Almere
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kakali\Documents\funda\fundanl\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4095"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14388" windowHeight="4092"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +53,6 @@
     <t>12 juni 2018 om 16:30 uur</t>
   </si>
   <si>
-    <t>No Updates Yet</t>
-  </si>
-  <si>
     <t>Home Location</t>
   </si>
   <si>
@@ -171,12 +173,15 @@
   </si>
   <si>
     <t>1313 AZ Almere</t>
+  </si>
+  <si>
+    <t>14 juni 2018 om 12:30 uur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -592,7 +597,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -603,46 +608,46 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" customWidth="1"/>
-    <col min="6" max="6" width="75.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" customWidth="1"/>
+    <col min="6" max="6" width="75.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
       <c r="C1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -656,7 +661,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -671,10 +676,10 @@
         <v>6</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -682,19 +687,19 @@
         <v>200</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -709,10 +714,10 @@
         <v>8</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -728,27 +733,27 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="8">
         <v>200</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="7">
         <v>215</v>
@@ -761,12 +766,12 @@
         <v>1</v>
       </c>
       <c r="F10" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="B11" s="2">
         <v>200</v>
@@ -779,12 +784,12 @@
         <v>1</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="6">
         <v>225</v>
@@ -794,61 +799,61 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="6">
         <v>210</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="5" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="B14" s="11">
         <v>190</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="2">
         <v>200</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>2</v>
@@ -857,18 +862,18 @@
         <v>1</v>
       </c>
       <c r="F15" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="B16" s="2">
         <v>200</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>2</v>
@@ -877,27 +882,27 @@
         <v>1</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="10">
         <v>225</v>
       </c>
       <c r="C17" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>9</v>
-      </c>
       <c r="F17" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Count Basiestraat 52
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kakali\Documents\funda\fundanl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Karnan\funda\fundanl\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -176,6 +176,18 @@
   </si>
   <si>
     <t>14 juni 2018 om 12:30 uur</t>
+  </si>
+  <si>
+    <t>Count Basiestraat 52</t>
+  </si>
+  <si>
+    <t>1311 PD Almere</t>
+  </si>
+  <si>
+    <t>No Updates yet</t>
+  </si>
+  <si>
+    <t>https://www.funda.nl/koop/almere/huis-40693517-count-basiestraat-52/</t>
   </si>
 </sst>
 </file>
@@ -351,7 +363,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -403,7 +415,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -605,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -903,6 +915,26 @@
       </c>
       <c r="F17" s="5" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="10">
+        <v>229500</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated remarks and new colours
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -200,6 +200,18 @@
   </si>
   <si>
     <t>1323 PS Almere</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>Seen, Not interested</t>
+  </si>
+  <si>
+    <t>Already Seen</t>
   </si>
 </sst>
 </file>
@@ -238,7 +250,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,6 +272,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -314,6 +332,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -629,29 +653,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="22.109375" customWidth="1"/>
     <col min="5" max="5" width="34.88671875" customWidth="1"/>
-    <col min="6" max="6" width="75.88671875" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="75.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="12"/>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C1" s="1"/>
+      <c r="D1" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -667,11 +695,12 @@
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -683,9 +712,14 @@
       <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -699,31 +733,35 @@
       <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="14">
         <v>200</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D6" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -737,11 +775,12 @@
       <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="1"/>
+      <c r="G7" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -755,13 +794,14 @@
       <c r="E8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" s="3"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>200</v>
       </c>
       <c r="C9" s="8"/>
@@ -771,11 +811,12 @@
       <c r="E9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="3"/>
+      <c r="G9" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -789,15 +830,16 @@
       <c r="E10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="3"/>
+      <c r="G10" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="7">
         <v>200</v>
       </c>
       <c r="C11" s="2"/>
@@ -807,11 +849,12 @@
       <c r="E11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="3"/>
+      <c r="G11" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -825,11 +868,12 @@
       <c r="E12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="1"/>
+      <c r="G12" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>26</v>
       </c>
@@ -845,11 +889,12 @@
       <c r="E13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="1"/>
+      <c r="G13" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>30</v>
       </c>
@@ -865,15 +910,16 @@
       <c r="E14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="1"/>
+      <c r="G14" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="7">
         <v>200</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -885,15 +931,16 @@
       <c r="E15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="3"/>
+      <c r="G15" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="7">
         <v>200</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -905,11 +952,12 @@
       <c r="E16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="3"/>
+      <c r="G16" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>45</v>
       </c>
@@ -925,11 +973,12 @@
       <c r="E17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>48</v>
       </c>
@@ -945,11 +994,12 @@
       <c r="E18" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="10"/>
+      <c r="G18" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>53</v>
       </c>
@@ -965,28 +1015,29 @@
       <c r="E19" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F9" r:id="rId1"/>
-    <hyperlink ref="F5" r:id="rId2"/>
-    <hyperlink ref="F6" r:id="rId3"/>
-    <hyperlink ref="F7" r:id="rId4"/>
-    <hyperlink ref="F10" r:id="rId5"/>
-    <hyperlink ref="F11" r:id="rId6"/>
-    <hyperlink ref="F12" r:id="rId7"/>
-    <hyperlink ref="F14" r:id="rId8"/>
-    <hyperlink ref="F15" r:id="rId9"/>
-    <hyperlink ref="F16" r:id="rId10"/>
-    <hyperlink ref="F19" r:id="rId11"/>
+    <hyperlink ref="G9" r:id="rId1"/>
+    <hyperlink ref="G5" r:id="rId2"/>
+    <hyperlink ref="G6" r:id="rId3"/>
+    <hyperlink ref="G7" r:id="rId4"/>
+    <hyperlink ref="G10" r:id="rId5"/>
+    <hyperlink ref="G11" r:id="rId6"/>
+    <hyperlink ref="G12" r:id="rId7"/>
+    <hyperlink ref="G14" r:id="rId8"/>
+    <hyperlink ref="G15" r:id="rId9"/>
+    <hyperlink ref="G16" r:id="rId10"/>
+    <hyperlink ref="G19" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>

</xml_diff>

<commit_message>
Added Johannes Vermeerstraat 165
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -190,9 +190,6 @@
     <t>https://www.funda.nl/koop/almere/huis-40693517-count-basiestraat-52/</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Moessorgskystraat 22</t>
   </si>
   <si>
@@ -222,6 +219,36 @@
   </si>
   <si>
     <t>https://www.funda.nl/koop/almere/huis-86010123-zeistpad-8/</t>
+  </si>
+  <si>
+    <t>Koolzaadweg 53</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1313 GK Almere
+</t>
+  </si>
+  <si>
+    <t>https://www.funda.nl/koop/almere/huis-40532360-koolzaadweg-53/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dwerggrashof 9
+</t>
+  </si>
+  <si>
+    <t>1313 AT Almere</t>
+  </si>
+  <si>
+    <t>https://www.funda.nl/koop/almere/huis-40694705-dwerggrashof-9/</t>
+  </si>
+  <si>
+    <t>Johannes Vermeerstraat 165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1318 HS Almere
+</t>
+  </si>
+  <si>
+    <t>https://www.funda.nl/koop/almere/huis-40670575-johannes-vermeerstraat-165/</t>
   </si>
 </sst>
 </file>
@@ -665,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,7 +713,7 @@
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -723,10 +750,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -765,7 +792,7 @@
         <v>34</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>18</v>
@@ -1011,13 +1038,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="6">
         <v>210</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>2</v>
@@ -1027,18 +1054,18 @@
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="6">
         <v>199500</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>2</v>
@@ -1048,37 +1075,71 @@
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="6"/>
+      <c r="B21" s="1">
+        <v>200</v>
+      </c>
       <c r="C21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="G21" s="5" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="1">
+        <v>200</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="1">
+        <v>225</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="G23" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
@@ -1120,8 +1181,9 @@
     <hyperlink ref="G15" r:id="rId9"/>
     <hyperlink ref="G16" r:id="rId10"/>
     <hyperlink ref="G19" r:id="rId11"/>
+    <hyperlink ref="G23" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Anna Pavlovastraat 4 and  Stan -- added
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Karnan\funda\fundanl\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14388" windowHeight="4092"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4095"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -249,12 +244,33 @@
   </si>
   <si>
     <t>https://www.funda.nl/koop/almere/huis-40670575-johannes-vermeerstraat-165/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stan Laurelstraat 31
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1325 CT Almere
+</t>
+  </si>
+  <si>
+    <t>https://www.funda.nl/koop/almere/huis-40695478-stan-laurelstraat-31/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anna Pavlovastraat 4
+</t>
+  </si>
+  <si>
+    <t>1326 TK Almere</t>
+  </si>
+  <si>
+    <t>https://www.funda.nl/koop/almere/huis-47220780-anna-pavlovastraat-4/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -347,7 +363,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -375,6 +391,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -436,7 +455,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -488,7 +507,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -682,7 +701,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -692,22 +711,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:F23"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="75.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="75.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" s="12" t="s">
         <v>36</v>
       </c>
@@ -716,7 +735,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -737,7 +756,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -756,7 +775,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -775,7 +794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>4</v>
       </c>
@@ -798,7 +817,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -817,7 +836,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -834,7 +853,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -853,7 +872,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -872,7 +891,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -891,7 +910,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -910,7 +929,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>26</v>
       </c>
@@ -931,7 +950,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>30</v>
       </c>
@@ -952,7 +971,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
@@ -973,7 +992,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
@@ -994,7 +1013,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>45</v>
       </c>
@@ -1015,7 +1034,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>48</v>
       </c>
@@ -1036,7 +1055,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>52</v>
       </c>
@@ -1057,7 +1076,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>59</v>
       </c>
@@ -1078,11 +1097,11 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="6">
         <v>200</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1099,11 +1118,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="6">
         <v>200</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1120,11 +1139,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="6">
         <v>225</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1141,25 +1160,49 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="6">
+        <v>235</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="10">
+        <v>225</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="6"/>
       <c r="C26" s="1"/>

</xml_diff>

<commit_message>
Updated Stan Laurelstraat 31
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -278,9 +278,6 @@
     <t>this property is sold with reservation.</t>
   </si>
   <si>
-    <t>June 12th 15:30:00</t>
-  </si>
-  <si>
     <t>June 19th 4PM to 5PM</t>
   </si>
   <si>
@@ -329,6 +326,9 @@
   </si>
   <si>
     <t>June 12 11AM</t>
+  </si>
+  <si>
+    <t>June 12th 15:45:00</t>
   </si>
 </sst>
 </file>
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,7 +816,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>11</v>
@@ -860,7 +860,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>6</v>
@@ -884,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>34</v>
@@ -908,7 +908,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
@@ -1016,7 +1016,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>33</v>
@@ -1040,7 +1040,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>37</v>
@@ -1064,7 +1064,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>33</v>
@@ -1136,7 +1136,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>47</v>
@@ -1160,10 +1160,10 @@
         <v>2</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="5" t="s">
@@ -1184,10 +1184,10 @@
         <v>2</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="5" t="s">
@@ -1256,10 +1256,10 @@
         <v>2</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1" t="s">
@@ -1304,10 +1304,10 @@
         <v>2</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="1" t="s">
@@ -1340,37 +1340,37 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B26" s="18">
         <v>219500</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B27" s="10">
         <v>215000</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>2</v>
@@ -1379,11 +1379,11 @@
         <v>50</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Kapitein de Langestraat 142
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="96">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>June 12th 15:45:00</t>
+  </si>
+  <si>
+    <t>Will be SOLD OUT</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -445,9 +448,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -459,6 +459,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -776,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,14 +801,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C1" s="1"/>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="16"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -871,28 +879,28 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <v>200</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="13" t="s">
+      <c r="D6" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1027,7 +1035,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="6">
@@ -1051,23 +1059,23 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="20">
         <v>190</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>33</v>
+      <c r="F14" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="9" t="s">
@@ -1290,11 +1298,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="17">
         <v>235</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -1306,10 +1314,10 @@
       <c r="E24" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="G24" s="17"/>
+      <c r="G24" s="16"/>
       <c r="H24" s="1" t="s">
         <v>73</v>
       </c>
@@ -1318,7 +1326,7 @@
       <c r="A25" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="17">
         <v>225</v>
       </c>
       <c r="C25" s="10" t="s">
@@ -1342,7 +1350,7 @@
       <c r="A26" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="17">
         <v>219500</v>
       </c>
       <c r="C26" s="10" t="s">

</xml_diff>

<commit_message>
Updated Boven Wijde 4
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="108">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Nat King Colestraat 24 Almere</t>
-  </si>
-  <si>
-    <t>13 juni 2018 at 16:00 hours</t>
   </si>
   <si>
     <t>Aarstraat 8 Almere</t>
@@ -464,7 +461,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -517,6 +514,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -836,7 +836,7 @@
       <pane xSplit="5" ySplit="12" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" sqref="A1:XFD3"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,42 +854,42 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="22"/>
       <c r="E1" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F1" s="15"/>
     </row>
     <row r="3" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="H3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -909,37 +909,37 @@
         <v>1</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="24">
         <v>200</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>6</v>
+      <c r="C5" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -950,23 +950,23 @@
         <v>200</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="12" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -977,7 +977,7 @@
         <v>225</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" s="20">
         <v>88</v>
@@ -986,19 +986,19 @@
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="7">
         <v>200</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="7">
         <v>200</v>
@@ -1027,7 +1027,7 @@
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>1</v>
@@ -1037,12 +1037,12 @@
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="7">
         <v>215</v>
@@ -1060,12 +1060,12 @@
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="7">
         <v>200</v>
@@ -1083,12 +1083,12 @@
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="6">
         <v>225</v>
@@ -1101,25 +1101,25 @@
         <v>2</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="20">
         <v>210</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="20">
         <v>106</v>
@@ -1128,50 +1128,50 @@
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="18">
         <v>190</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="19" t="s">
         <v>2</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="7">
         <v>200</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="2" t="s">
@@ -1185,18 +1185,18 @@
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="7">
         <v>200</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="2" t="s">
@@ -1210,18 +1210,18 @@
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="6">
         <v>225</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="16">
         <v>122</v>
@@ -1230,25 +1230,25 @@
         <v>2</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="6">
         <v>229500</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="16">
         <v>115</v>
@@ -1257,25 +1257,25 @@
         <v>2</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="6">
         <v>210</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" s="16">
         <v>106</v>
@@ -1284,25 +1284,25 @@
         <v>2</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="7">
         <v>199500</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="2" t="s">
@@ -1316,18 +1316,18 @@
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="7">
         <v>200</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="2" t="s">
@@ -1337,22 +1337,22 @@
         <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="6">
         <v>200</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" s="20">
         <v>111</v>
@@ -1361,27 +1361,27 @@
         <v>2</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" s="7">
         <v>225</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="2" t="s">
@@ -1395,18 +1395,18 @@
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B24" s="20">
         <v>235</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D24" s="20">
         <v>111</v>
@@ -1415,25 +1415,25 @@
         <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="20">
         <v>225</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D25" s="20">
         <v>115</v>
@@ -1442,50 +1442,50 @@
         <v>2</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B26" s="20">
         <v>219500</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B27" s="20">
         <v>215000</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D27" s="20">
         <v>105</v>
@@ -1494,25 +1494,25 @@
         <v>2</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B28" s="7">
         <v>225</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D28" s="7">
         <v>123</v>
@@ -1528,18 +1528,18 @@
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>102</v>
       </c>
       <c r="B29" s="12">
         <v>215</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D29" s="12">
         <v>105</v>
@@ -1548,41 +1548,43 @@
         <v>2</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="3">
+        <v>260</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B30" s="20">
-        <v>260</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D30" s="20">
+      <c r="D30" s="3">
         <v>148</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G30" s="1"/>
+      <c r="E30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Marty Feldmanstraat 61
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="112">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -363,6 +363,19 @@
   </si>
   <si>
     <t>https://www.funda.nl/koop/almere/huis-40688711-schonbergweg-31/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marty Feldmanstraat 61
+</t>
+  </si>
+  <si>
+    <t>1325 GL Almere</t>
+  </si>
+  <si>
+    <t>https://www.funda.nl/koop/almere/huis-40606409-marty-feldmanstraat-61/</t>
+  </si>
+  <si>
+    <t>June 20 2018 16:00 - 17:00 - Open House</t>
   </si>
 </sst>
 </file>
@@ -833,10 +846,10 @@
   <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="12" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="12" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:E5"/>
+      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,15 +1601,31 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="1">
+        <v>225</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" s="1">
+        <v>124</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
+      <c r="I31" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
@@ -2281,6 +2310,7 @@
       <c r="I93" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A3:I30"/>
   <hyperlinks>
     <hyperlink ref="I9" r:id="rId1"/>
     <hyperlink ref="I5" r:id="rId2"/>

</xml_diff>

<commit_message>
Added Count Basiestraat 48
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -11,9 +11,10 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$I$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$I$34</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -291,9 +292,6 @@
     <t>https://www.funda.nl/koop/almere/huis-86033952-rumbastraat-75/</t>
   </si>
   <si>
-    <t>Salsastraat 183</t>
-  </si>
-  <si>
     <t xml:space="preserve">1326 LW Almere
 </t>
   </si>
@@ -307,9 +305,6 @@
     <t>App Not Possible</t>
   </si>
   <si>
-    <t>June 12 11AM</t>
-  </si>
-  <si>
     <t>June 12th 15:45:00</t>
   </si>
   <si>
@@ -429,6 +424,12 @@
   </si>
   <si>
     <t>https://www.funda.nl/koop/almere/huis-40651733-hildebrandstraat-15/</t>
+  </si>
+  <si>
+    <t>Count Basiestraat 48</t>
+  </si>
+  <si>
+    <t>https://www.funda.nl/koop/almere/huis-40692235-count-basiestraat-48/</t>
   </si>
 </sst>
 </file>
@@ -597,9 +598,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -608,6 +606,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -618,9 +619,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -915,7 +913,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -923,10 +921,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I93"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:I35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +941,7 @@
     <col min="9" max="9" width="75.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="25" t="s">
         <v>35</v>
       </c>
@@ -953,7 +952,7 @@
       </c>
       <c r="F1" s="14"/>
     </row>
-    <row r="3" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -964,7 +963,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>9</v>
@@ -982,7 +981,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +1004,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>3</v>
       </c>
@@ -1013,10 +1012,10 @@
         <v>200</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>2</v>
@@ -1032,7 +1031,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
@@ -1059,7 +1058,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>5</v>
       </c>
@@ -1067,7 +1066,7 @@
         <v>225</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D7" s="27">
         <v>88</v>
@@ -1082,13 +1081,13 @@
         <v>7</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1109,7 +1108,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1132,7 +1131,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1155,7 +1154,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1248,14 +1247,14 @@
         <v>81</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
@@ -1280,7 +1279,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1305,7 +1304,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>44</v>
       </c>
@@ -1325,14 +1324,14 @@
         <v>79</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>46</v>
       </c>
@@ -1360,16 +1359,16 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="29">
         <v>210</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="30">
         <v>106</v>
       </c>
       <c r="E19" s="16" t="s">
@@ -1382,13 +1381,13 @@
         <v>77</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>57</v>
       </c>
@@ -1413,7 +1412,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>60</v>
       </c>
@@ -1438,7 +1437,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -1458,16 +1457,16 @@
         <v>79</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>66</v>
       </c>
@@ -1492,34 +1491,36 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="27">
         <v>235</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="27">
         <v>111</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="E24" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H24" s="1"/>
+      <c r="G24" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>55</v>
+      </c>
       <c r="I24" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -1546,7 +1547,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>82</v>
       </c>
@@ -1561,138 +1562,138 @@
         <v>2</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="7">
+        <v>225</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="7">
+        <v>123</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="26">
+        <v>215</v>
+      </c>
+      <c r="C28" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="19">
-        <v>215000</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="D28" s="26">
+        <v>105</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="H28" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D27" s="19">
+    </row>
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="3">
+        <v>260</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="3">
+        <v>148</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="6">
+        <v>225</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="7">
-        <v>225</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="7">
-        <v>123</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
-      <c r="A29" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="B29" s="26">
-        <v>215</v>
-      </c>
-      <c r="C29" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="26">
-        <v>105</v>
-      </c>
-      <c r="E29" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F29" s="26" t="s">
+      <c r="D30" s="1">
+        <v>124</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G29" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="H29" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="3">
-        <v>260</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="3">
-        <v>148</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>1</v>
+      <c r="G30" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B31" s="1">
-        <v>225</v>
+        <v>109</v>
+      </c>
+      <c r="B31" s="6">
+        <v>179</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D31" s="1">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>2</v>
@@ -1701,52 +1702,50 @@
         <v>79</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B32" s="1">
-        <v>179</v>
+        <v>112</v>
+      </c>
+      <c r="B32" s="6">
+        <v>195</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D32" s="1">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B33" s="1">
-        <v>195</v>
+        <v>120</v>
+      </c>
+      <c r="B33" s="6">
+        <v>225</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D33" s="1">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>2</v>
@@ -1757,18 +1756,18 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B34" s="1">
+        <v>123</v>
+      </c>
+      <c r="B34" s="6">
         <v>225</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D34" s="1">
         <v>107</v>
@@ -1782,21 +1781,21 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B35" s="1">
-        <v>225</v>
-      </c>
-      <c r="C35" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D35" s="1">
-        <v>107</v>
+      <c r="B35" s="6">
+        <v>200</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="19">
+        <v>115</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>2</v>
@@ -2437,19 +2436,18 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-      <c r="B93" s="19"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="19"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A3:I3"/>
+  <autoFilter ref="A3:I34">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="App Not Possible"/>
+        <filter val="Appt Not Possible"/>
+        <filter val="Completed"/>
+        <filter val="No Updates yet"/>
+        <filter val="YES"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="I9" r:id="rId1"/>
     <hyperlink ref="I5" r:id="rId2"/>
@@ -2464,13 +2462,12 @@
     <hyperlink ref="I23" r:id="rId11"/>
     <hyperlink ref="I27" r:id="rId12"/>
     <hyperlink ref="I28" r:id="rId13"/>
-    <hyperlink ref="I29" r:id="rId14"/>
-    <hyperlink ref="I19" r:id="rId15"/>
-    <hyperlink ref="I32" r:id="rId16"/>
-    <hyperlink ref="I17" r:id="rId17"/>
+    <hyperlink ref="I19" r:id="rId14"/>
+    <hyperlink ref="I31" r:id="rId15"/>
+    <hyperlink ref="I17" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
@@ -2485,8 +2482,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>121</v>
+      <c r="A2" s="31" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the Updtes feild
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Karnan\funda\fundanl\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4095"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14388" windowHeight="4092"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="153">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -396,9 +401,6 @@
     <t>June 23 10.00AM</t>
   </si>
   <si>
-    <t>Reject</t>
-  </si>
-  <si>
     <t>Bid form sent for 230100, SOLD OUT</t>
   </si>
   <si>
@@ -499,12 +501,27 @@
   </si>
   <si>
     <t>https://www.funda.nl/koop/almere/huis-40603144-enschedepad-62/</t>
+  </si>
+  <si>
+    <t>June 20 2018 10:45AM</t>
+  </si>
+  <si>
+    <t>called no response</t>
+  </si>
+  <si>
+    <t>SOLDOUT</t>
+  </si>
+  <si>
+    <t>owner will call back</t>
+  </si>
+  <si>
+    <t>Contacted helpdesk, they arrange to view</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -610,7 +627,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -628,10 +645,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -643,9 +656,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -678,6 +688,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -688,6 +701,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -982,7 +998,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -992,45 +1008,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:I41"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="24" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" style="21" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="24" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" customWidth="1"/>
     <col min="7" max="7" width="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="75.85546875" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="75.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="22" t="s">
         <v>35</v>
       </c>
       <c r="C1" s="1"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="14" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="14"/>
-    </row>
-    <row r="3" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="12"/>
+    </row>
+    <row r="3" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="19" t="s">
         <v>99</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1049,7 +1065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1072,20 +1088,20 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="20">
         <v>200</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -1099,63 +1115,63 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="24">
         <v>200</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="24">
         <v>225</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="24">
         <v>88</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="26" t="s">
+      <c r="E7" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="26" t="s">
-        <v>117</v>
+      <c r="H7" s="23" t="s">
+        <v>55</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1176,7 +1192,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1199,7 +1215,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1222,7 +1238,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1245,7 +1261,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1270,17 +1286,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="17">
         <v>210</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="17">
         <v>106</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1297,24 +1313,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="15">
         <v>190</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="18" t="s">
+      <c r="D14" s="20"/>
+      <c r="E14" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="16" t="s">
         <v>90</v>
       </c>
       <c r="H14" s="1"/>
@@ -1322,7 +1338,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
@@ -1347,7 +1363,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1372,7 +1388,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>44</v>
       </c>
@@ -1382,7 +1398,7 @@
       <c r="C17" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="13">
         <v>122</v>
       </c>
       <c r="E17" s="10" t="s">
@@ -1399,7 +1415,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>46</v>
       </c>
@@ -1409,7 +1425,7 @@
       <c r="C18" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="13">
         <v>115</v>
       </c>
       <c r="E18" s="10" t="s">
@@ -1426,36 +1442,36 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="25">
         <v>210</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="26">
         <v>106</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="16" t="s">
+      <c r="E19" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="H19" s="16" t="s">
-        <v>118</v>
+      <c r="H19" s="14" t="s">
+        <v>117</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>57</v>
       </c>
@@ -1480,7 +1496,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>60</v>
       </c>
@@ -1505,7 +1521,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -1515,7 +1531,7 @@
       <c r="C22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="17">
         <v>111</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -1534,7 +1550,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>66</v>
       </c>
@@ -1559,46 +1575,46 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="27">
+      <c r="B24" s="24">
         <v>235</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D24" s="24">
         <v>111</v>
       </c>
-      <c r="E24" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" s="26" t="s">
+      <c r="E24" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="G24" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="H24" s="26" t="s">
+      <c r="H24" s="23" t="s">
         <v>55</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="17">
         <v>225</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="17">
         <v>115</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -1608,24 +1624,24 @@
         <v>48</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>48</v>
+        <v>151</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="17">
         <v>219500</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D26" s="19"/>
+      <c r="D26" s="17"/>
       <c r="E26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1640,7 +1656,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>94</v>
       </c>
@@ -1667,40 +1683,40 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
+    <row r="28" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="26">
+      <c r="B28" s="24">
         <v>215</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="23">
         <v>105</v>
       </c>
-      <c r="E28" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F28" s="26" t="s">
+      <c r="E28" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="G28" s="26" t="s">
+      <c r="G28" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="H28" s="26" t="s">
+      <c r="H28" s="23" t="s">
         <v>55</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="30">
         <v>260</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1723,7 +1739,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>104</v>
       </c>
@@ -1750,7 +1766,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>109</v>
       </c>
@@ -1777,7 +1793,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>112</v>
       </c>
@@ -1794,23 +1810,25 @@
         <v>2</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G32" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>148</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B33" s="6">
         <v>225</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D33" s="1">
         <v>107</v>
@@ -1824,18 +1842,18 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="B34" s="6">
         <v>225</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D34" s="1">
         <v>107</v>
@@ -1843,26 +1861,26 @@
       <c r="E34" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="B35" s="6">
         <v>200</v>
       </c>
-      <c r="C35" s="31" t="s">
+      <c r="C35" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D35" s="17">
         <v>115</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -1871,21 +1889,23 @@
       <c r="F35" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="29" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
+      <c r="B36" s="17">
+        <v>300</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="B36" s="1">
-        <v>300</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="D36" s="1">
         <v>138</v>
@@ -1899,18 +1919,18 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="17">
+        <v>213700</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B37" s="1">
-        <v>213700</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="D37" s="1">
         <v>103</v>
@@ -1924,18 +1944,18 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="B38" s="17">
+        <v>259500</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B38" s="1">
-        <v>259500</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="D38" s="1">
         <v>104</v>
@@ -1949,18 +1969,18 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="17">
+        <v>225</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B39" s="1">
-        <v>225</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="D39" s="1">
         <v>115</v>
@@ -1972,22 +1992,22 @@
         <v>79</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="17">
+        <v>250</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B40" s="1">
-        <v>250</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="D40" s="1">
         <v>130</v>
@@ -1996,596 +2016,598 @@
         <v>2</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G40" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="B41" s="17">
+        <v>185</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B41" s="1">
-        <v>185</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="D41" s="1">
         <v>126</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
-      <c r="B42" s="19"/>
+      <c r="B42" s="17"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="19"/>
+      <c r="D42" s="17"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
-      <c r="B43" s="19"/>
+      <c r="B43" s="17"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="19"/>
+      <c r="D43" s="17"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
-      <c r="B44" s="19"/>
+      <c r="B44" s="17"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="19"/>
+      <c r="D44" s="17"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
-      <c r="B45" s="19"/>
+      <c r="B45" s="17"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="19"/>
+      <c r="D45" s="17"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
-      <c r="B46" s="19"/>
+      <c r="B46" s="17"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="19"/>
+      <c r="D46" s="17"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
-      <c r="B47" s="19"/>
+      <c r="B47" s="17"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="19"/>
+      <c r="D47" s="17"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
-      <c r="B48" s="19"/>
+      <c r="B48" s="17"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="19"/>
+      <c r="D48" s="17"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
-      <c r="B49" s="19"/>
+      <c r="B49" s="17"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="19"/>
+      <c r="D49" s="17"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
-      <c r="B50" s="19"/>
+      <c r="B50" s="17"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="19"/>
+      <c r="D50" s="17"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
-      <c r="B51" s="19"/>
+      <c r="B51" s="17"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="19"/>
+      <c r="D51" s="17"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
-      <c r="B52" s="19"/>
+      <c r="B52" s="17"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="19"/>
+      <c r="D52" s="17"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
-      <c r="B53" s="19"/>
+      <c r="B53" s="17"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="19"/>
+      <c r="D53" s="17"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
-      <c r="B54" s="19"/>
+      <c r="B54" s="17"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="19"/>
+      <c r="D54" s="17"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
-      <c r="B55" s="19"/>
+      <c r="B55" s="17"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="19"/>
+      <c r="D55" s="17"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
-      <c r="B56" s="19"/>
+      <c r="B56" s="17"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="19"/>
+      <c r="D56" s="17"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
-      <c r="B57" s="19"/>
+      <c r="B57" s="17"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="19"/>
+      <c r="D57" s="17"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
-      <c r="B58" s="19"/>
+      <c r="B58" s="17"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="19"/>
+      <c r="D58" s="17"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
-      <c r="B59" s="19"/>
+      <c r="B59" s="17"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="19"/>
+      <c r="D59" s="17"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
-      <c r="B60" s="19"/>
+      <c r="B60" s="17"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="19"/>
+      <c r="D60" s="17"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
-      <c r="B61" s="19"/>
+      <c r="B61" s="17"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="19"/>
+      <c r="D61" s="17"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
-      <c r="B62" s="19"/>
+      <c r="B62" s="17"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="19"/>
+      <c r="D62" s="17"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
-      <c r="B63" s="19"/>
+      <c r="B63" s="17"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="19"/>
+      <c r="D63" s="17"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
-      <c r="B64" s="19"/>
+      <c r="B64" s="17"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="19"/>
+      <c r="D64" s="17"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
-      <c r="B65" s="19"/>
+      <c r="B65" s="17"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="19"/>
+      <c r="D65" s="17"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
-      <c r="B66" s="19"/>
+      <c r="B66" s="17"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="19"/>
+      <c r="D66" s="17"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
-      <c r="B67" s="19"/>
+      <c r="B67" s="17"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="19"/>
+      <c r="D67" s="17"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
-      <c r="B68" s="19"/>
+      <c r="B68" s="17"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="19"/>
+      <c r="D68" s="17"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
-      <c r="B69" s="19"/>
+      <c r="B69" s="17"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="19"/>
+      <c r="D69" s="17"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
-      <c r="B70" s="19"/>
+      <c r="B70" s="17"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="19"/>
+      <c r="D70" s="17"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
-      <c r="B71" s="19"/>
+      <c r="B71" s="17"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="19"/>
+      <c r="D71" s="17"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
-      <c r="B72" s="19"/>
+      <c r="B72" s="17"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="19"/>
+      <c r="D72" s="17"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
-      <c r="B73" s="19"/>
+      <c r="B73" s="17"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="19"/>
+      <c r="D73" s="17"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
-      <c r="B74" s="19"/>
+      <c r="B74" s="17"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="19"/>
+      <c r="D74" s="17"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
-      <c r="B75" s="19"/>
+      <c r="B75" s="17"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="19"/>
+      <c r="D75" s="17"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
-      <c r="B76" s="19"/>
+      <c r="B76" s="17"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="19"/>
+      <c r="D76" s="17"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
-      <c r="B77" s="19"/>
+      <c r="B77" s="17"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="19"/>
+      <c r="D77" s="17"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
-      <c r="B78" s="19"/>
+      <c r="B78" s="17"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="19"/>
+      <c r="D78" s="17"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
-      <c r="B79" s="19"/>
+      <c r="B79" s="17"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="19"/>
+      <c r="D79" s="17"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
-      <c r="B80" s="19"/>
+      <c r="B80" s="17"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="19"/>
+      <c r="D80" s="17"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
-      <c r="B81" s="19"/>
+      <c r="B81" s="17"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="19"/>
+      <c r="D81" s="17"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
-      <c r="B82" s="19"/>
+      <c r="B82" s="17"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="19"/>
+      <c r="D82" s="17"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
-      <c r="B83" s="19"/>
+      <c r="B83" s="17"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="19"/>
+      <c r="D83" s="17"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
-      <c r="B84" s="19"/>
+      <c r="B84" s="17"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="19"/>
+      <c r="D84" s="17"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
-      <c r="B85" s="19"/>
+      <c r="B85" s="17"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="19"/>
+      <c r="D85" s="17"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
-      <c r="B86" s="19"/>
+      <c r="B86" s="17"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="19"/>
+      <c r="D86" s="17"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
-      <c r="B87" s="19"/>
+      <c r="B87" s="17"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="19"/>
+      <c r="D87" s="17"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
-      <c r="B88" s="19"/>
+      <c r="B88" s="17"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="19"/>
+      <c r="D88" s="17"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
-      <c r="B89" s="19"/>
+      <c r="B89" s="17"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="19"/>
+      <c r="D89" s="17"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
-      <c r="B90" s="19"/>
+      <c r="B90" s="17"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="19"/>
+      <c r="D90" s="17"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
-      <c r="B91" s="19"/>
+      <c r="B91" s="17"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="19"/>
+      <c r="D91" s="17"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
-      <c r="B92" s="19"/>
+      <c r="B92" s="17"/>
       <c r="C92" s="1"/>
-      <c r="D92" s="19"/>
+      <c r="D92" s="17"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
@@ -2625,11 +2647,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>119</v>
+    <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2645,7 +2667,7 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Rodinweg 51 with the new viewing date
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -516,9 +516,6 @@
     <t>https://www.funda.nl/koop/almere/huis-40609020-valetaweg-91/</t>
   </si>
   <si>
-    <t>22 June 9:15am</t>
-  </si>
-  <si>
     <t>23 June 10AM to 11:30</t>
   </si>
   <si>
@@ -541,6 +538,9 @@
   </si>
   <si>
     <t>27 June 17:00</t>
+  </si>
+  <si>
+    <t>22 June 8:50am</t>
   </si>
 </sst>
 </file>
@@ -652,7 +652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -709,10 +709,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1030,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1457,7 +1463,7 @@
         <v>77</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="5" t="s">
@@ -1544,28 +1550,28 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="31">
         <v>200</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="24">
         <v>111</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22" s="10" t="s">
+      <c r="E22" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="23" t="s">
         <v>91</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -1738,7 +1744,7 @@
       <c r="A29" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="28">
+      <c r="B29" s="29">
         <v>260</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1762,7 +1768,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="28" t="s">
         <v>102</v>
       </c>
       <c r="B30" s="6">
@@ -1781,7 +1787,7 @@
         <v>77</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1" t="s">
@@ -1808,7 +1814,7 @@
         <v>77</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
@@ -1835,7 +1841,7 @@
         <v>77</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1" t="s">
@@ -1926,7 +1932,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="30" t="s">
         <v>123</v>
       </c>
       <c r="B36" s="20">
@@ -1972,7 +1978,7 @@
         <v>77</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
@@ -1999,7 +2005,7 @@
         <v>77</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="5" t="s">
@@ -2026,7 +2032,7 @@
         <v>77</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="5" t="s">
@@ -2080,7 +2086,7 @@
         <v>77</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="5" t="s">
@@ -2104,10 +2110,10 @@
         <v>2</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="5" t="s">
@@ -2118,7 +2124,7 @@
       <c r="A43" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="17">
         <v>22500</v>
       </c>
       <c r="C43" s="1" t="s">

</xml_diff>

<commit_message>
Updated Eikenstraat 54 with the new viewing date
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -534,13 +534,13 @@
     <t>25 June 16:30</t>
   </si>
   <si>
-    <t>25 June 14:00</t>
-  </si>
-  <si>
     <t>27 June 17:00</t>
   </si>
   <si>
     <t>22 June 8:50am</t>
+  </si>
+  <si>
+    <t>04 July 14:00</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1037,7 @@
   <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2005,7 +2005,7 @@
         <v>77</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="5" t="s">
@@ -2032,7 +2032,7 @@
         <v>77</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="5" t="s">
@@ -2113,7 +2113,7 @@
         <v>77</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="5" t="s">

</xml_diff>

<commit_message>
Updated Marty Feldmanstraat 61
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Karnan\funda\fundanl\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14388" windowHeight="4092"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4095"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="175">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -583,12 +578,15 @@
   </si>
   <si>
     <t>1313 CT Almere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery next year May </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -694,7 +692,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -760,6 +758,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1068,7 +1069,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1078,24 +1079,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" style="21" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="21" customWidth="1"/>
     <col min="3" max="3" width="15" style="21" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="21" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" customWidth="1"/>
     <col min="7" max="7" width="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="75.88671875" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="75.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" s="22" t="s">
         <v>34</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1158,7 +1159,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
@@ -1185,7 +1186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>4</v>
       </c>
@@ -1212,7 +1213,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>5</v>
       </c>
@@ -1241,7 +1242,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1262,7 +1263,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1285,7 +1286,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1308,7 +1309,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1331,7 +1332,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1358,7 +1359,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1385,7 +1386,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>29</v>
       </c>
@@ -1410,7 +1411,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1435,7 +1436,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -1460,7 +1461,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>43</v>
       </c>
@@ -1487,7 +1488,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
         <v>45</v>
       </c>
@@ -1516,7 +1517,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>49</v>
       </c>
@@ -1545,7 +1546,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>56</v>
       </c>
@@ -1570,7 +1571,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>59</v>
       </c>
@@ -1595,7 +1596,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="23" t="s">
         <v>62</v>
       </c>
@@ -1624,7 +1625,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>65</v>
       </c>
@@ -1649,7 +1650,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="23" t="s">
         <v>68</v>
       </c>
@@ -1678,7 +1679,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
@@ -1705,7 +1706,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
@@ -1730,7 +1731,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>90</v>
       </c>
@@ -1757,7 +1758,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>93</v>
       </c>
@@ -1786,7 +1787,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>97</v>
       </c>
@@ -1813,34 +1814,36 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="28" t="s">
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="31">
         <v>225</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="24">
         <v>124</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="E30" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="H30" s="1"/>
+      <c r="H30" s="23" t="s">
+        <v>174</v>
+      </c>
       <c r="I30" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>103</v>
       </c>
@@ -1867,7 +1870,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
         <v>106</v>
       </c>
@@ -1896,7 +1899,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>112</v>
       </c>
@@ -1923,7 +1926,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>115</v>
       </c>
@@ -1950,7 +1953,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>118</v>
       </c>
@@ -1979,7 +1982,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
         <v>120</v>
       </c>
@@ -2006,7 +2009,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>123</v>
       </c>
@@ -2033,7 +2036,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>126</v>
       </c>
@@ -2060,7 +2063,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>129</v>
       </c>
@@ -2087,7 +2090,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>132</v>
       </c>
@@ -2114,7 +2117,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>135</v>
       </c>
@@ -2143,7 +2146,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>142</v>
       </c>
@@ -2170,7 +2173,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>146</v>
       </c>
@@ -2195,7 +2198,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>160</v>
       </c>
@@ -2222,7 +2225,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>163</v>
       </c>
@@ -2249,7 +2252,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
         <v>168</v>
       </c>
@@ -2276,7 +2279,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
@@ -2287,7 +2290,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
@@ -2298,7 +2301,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
@@ -2309,7 +2312,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
@@ -2320,7 +2323,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
@@ -2331,7 +2334,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
@@ -2342,7 +2345,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
@@ -2353,7 +2356,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>
@@ -2364,7 +2367,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
@@ -2375,7 +2378,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
@@ -2386,7 +2389,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
@@ -2397,7 +2400,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
@@ -2408,7 +2411,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
@@ -2419,7 +2422,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
@@ -2430,7 +2433,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="17"/>
       <c r="C61" s="17"/>
@@ -2441,7 +2444,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="17"/>
       <c r="C62" s="17"/>
@@ -2452,7 +2455,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
@@ -2463,7 +2466,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="17"/>
       <c r="C64" s="17"/>
@@ -2474,7 +2477,7 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
@@ -2485,7 +2488,7 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="17"/>
       <c r="C66" s="17"/>
@@ -2496,7 +2499,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="17"/>
       <c r="C67" s="17"/>
@@ -2507,7 +2510,7 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>
@@ -2518,7 +2521,7 @@
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="17"/>
       <c r="C69" s="17"/>
@@ -2529,7 +2532,7 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="17"/>
       <c r="C70" s="17"/>
@@ -2540,7 +2543,7 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="17"/>
       <c r="C71" s="17"/>
@@ -2551,7 +2554,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="17"/>
       <c r="C72" s="17"/>
@@ -2562,7 +2565,7 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="17"/>
       <c r="C73" s="17"/>
@@ -2573,7 +2576,7 @@
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="17"/>
       <c r="C74" s="17"/>
@@ -2584,7 +2587,7 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="17"/>
       <c r="C75" s="17"/>
@@ -2595,7 +2598,7 @@
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="17"/>
       <c r="C76" s="17"/>
@@ -2606,7 +2609,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="17"/>
       <c r="C77" s="17"/>
@@ -2617,7 +2620,7 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="17"/>
       <c r="C78" s="17"/>
@@ -2628,7 +2631,7 @@
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="17"/>
       <c r="C79" s="17"/>
@@ -2639,7 +2642,7 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="17"/>
       <c r="C80" s="17"/>
@@ -2650,7 +2653,7 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="17"/>
       <c r="C81" s="17"/>
@@ -2661,7 +2664,7 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="17"/>
       <c r="C82" s="17"/>
@@ -2672,7 +2675,7 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="17"/>
       <c r="C83" s="17"/>
@@ -2683,7 +2686,7 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
@@ -2694,7 +2697,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="17"/>
       <c r="C85" s="17"/>
@@ -2705,7 +2708,7 @@
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="17"/>
       <c r="C86" s="17"/>
@@ -2716,7 +2719,7 @@
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="17"/>
       <c r="C87" s="17"/>
@@ -2727,7 +2730,7 @@
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="17"/>
       <c r="C88" s="17"/>
@@ -2738,7 +2741,7 @@
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="17"/>
       <c r="C89" s="17"/>
@@ -2749,7 +2752,7 @@
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="17"/>
       <c r="C90" s="17"/>
@@ -2760,7 +2763,7 @@
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="17"/>
       <c r="C91" s="17"/>
@@ -2771,7 +2774,7 @@
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="17"/>
       <c r="C92" s="17"/>
@@ -2821,7 +2824,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
@@ -2841,7 +2844,7 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Erik Satiestraat 22
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="179">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -581,6 +581,18 @@
   </si>
   <si>
     <t xml:space="preserve">Delivery next year May </t>
+  </si>
+  <si>
+    <t>Erik Satiestraat 22</t>
+  </si>
+  <si>
+    <t>https://www.funda.nl/koop/almere/huis-40619868-erik-satiestraat-22/</t>
+  </si>
+  <si>
+    <t>1323 SN Almere</t>
+  </si>
+  <si>
+    <t>03 July 4PM</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1081,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1079,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,29 +1372,31 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="23">
         <v>210</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="23">
         <v>106</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="E13" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1" t="s">
+      <c r="H13" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="23" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2147,28 +2161,30 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="B42" s="17">
+      <c r="B42" s="23">
         <v>192500</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="23">
         <v>77</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F42" s="1" t="s">
+      <c r="E42" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G42" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="H42" s="1"/>
+      <c r="H42" s="23" t="s">
+        <v>54</v>
+      </c>
       <c r="I42" s="5" t="s">
         <v>144</v>
       </c>
@@ -2280,15 +2296,31 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B47" s="1">
+        <v>235</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D47" s="1">
+        <v>114</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
+      <c r="I47" s="1" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>

</xml_diff>

<commit_message>
Updated June 22 viewing
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$I$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$I$47</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="180">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -593,6 +593,9 @@
   </si>
   <si>
     <t>03 July 4PM</t>
+  </si>
+  <si>
+    <t>See, Thinking</t>
   </si>
 </sst>
 </file>
@@ -638,7 +641,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -675,6 +678,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -704,7 +713,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -724,9 +733,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -773,6 +779,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1081,7 +1091,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1089,18 +1099,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="21" customWidth="1"/>
-    <col min="3" max="3" width="15" style="21" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="21" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="15" style="20" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="20" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" customWidth="1"/>
     <col min="7" max="7" width="37" bestFit="1" customWidth="1"/>
@@ -1109,11 +1120,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="18"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="12" t="s">
         <v>55</v>
       </c>
@@ -1123,13 +1134,13 @@
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>95</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1148,7 +1159,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1171,20 +1182,20 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>200</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="15" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -1198,63 +1209,63 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>200</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="23" t="s">
+      <c r="D6" s="23"/>
+      <c r="E6" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="22" t="s">
         <v>54</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+    <row r="7" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <v>225</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="23">
         <v>88</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="23" t="s">
+      <c r="E7" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="22" t="s">
         <v>54</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1275,7 +1286,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1298,7 +1309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1321,7 +1332,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1344,17 +1355,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="16">
         <v>225</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <v>109</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1372,52 +1383,52 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="23">
         <v>210</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <v>106</v>
       </c>
-      <c r="E13" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="23" t="s">
+      <c r="E13" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>190</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="16" t="s">
+      <c r="D14" s="19"/>
+      <c r="E14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="15" t="s">
         <v>86</v>
       </c>
       <c r="H14" s="1"/>
@@ -1425,7 +1436,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1450,7 +1461,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -1475,76 +1486,78 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="23">
         <v>225</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="22">
         <v>122</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="10" t="s">
+      <c r="E17" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="H17" s="10"/>
+      <c r="H17" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="I17" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
+    <row r="18" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="31">
+      <c r="B18" s="30">
         <v>229500</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="23">
         <v>115</v>
       </c>
-      <c r="E18" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="23" t="s">
+      <c r="E18" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="H18" s="23" t="s">
+      <c r="H18" s="22" t="s">
         <v>54</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="24">
         <v>210</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="25">
         <v>106</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>2</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -1553,14 +1566,14 @@
       <c r="G19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="13" t="s">
         <v>110</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>56</v>
       </c>
@@ -1585,7 +1598,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>59</v>
       </c>
@@ -1610,36 +1623,36 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A22" s="23" t="s">
+    <row r="22" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="31">
+      <c r="B22" s="30">
         <v>200</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="23">
         <v>111</v>
       </c>
-      <c r="E22" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22" s="23" t="s">
+      <c r="E22" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="H22" s="22" t="s">
         <v>145</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>65</v>
       </c>
@@ -1664,46 +1677,46 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A24" s="23" t="s">
+    <row r="24" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="24">
+      <c r="B24" s="23">
         <v>235</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="23">
         <v>111</v>
       </c>
-      <c r="E24" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" s="23" t="s">
+      <c r="E24" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="H24" s="23" t="s">
+      <c r="H24" s="22" t="s">
         <v>54</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="17">
+      <c r="B25" s="16">
         <v>225</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="16">
         <v>115</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -1720,17 +1733,17 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="17">
+      <c r="B26" s="16">
         <v>219500</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="17"/>
+      <c r="D26" s="16"/>
       <c r="E26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1745,7 +1758,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>90</v>
       </c>
@@ -1772,46 +1785,46 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+    <row r="28" spans="1:9" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="24">
+      <c r="B28" s="23">
         <v>215</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="23">
         <v>105</v>
       </c>
-      <c r="E28" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F28" s="23" t="s">
+      <c r="E28" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G28" s="23" t="s">
+      <c r="G28" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="H28" s="23" t="s">
+      <c r="H28" s="22" t="s">
         <v>54</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B29" s="29">
+      <c r="B29" s="28">
         <v>260</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="28">
         <v>148</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -1828,46 +1841,46 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
+    <row r="30" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="31">
+      <c r="B30" s="30">
         <v>225</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="23">
         <v>124</v>
       </c>
-      <c r="E30" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F30" s="23" t="s">
+      <c r="E30" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="23" t="s">
+      <c r="G30" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="H30" s="23" t="s">
+      <c r="H30" s="22" t="s">
         <v>174</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B31" s="6">
         <v>179</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="16">
         <v>99</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -1884,49 +1897,49 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="B32" s="24">
+      <c r="B32" s="23">
         <v>195</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="23">
         <v>80</v>
       </c>
-      <c r="E32" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F32" s="23" t="s">
+      <c r="E32" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G32" s="23" t="s">
+      <c r="G32" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="H32" s="23" t="s">
+      <c r="H32" s="22" t="s">
         <v>54</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B33" s="25">
+      <c r="B33" s="24">
         <v>225</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="D33" s="20">
+      <c r="D33" s="19">
         <v>107</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="15" t="s">
         <v>2</v>
       </c>
       <c r="F33" s="3" t="s">
@@ -1940,20 +1953,20 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="B34" s="25">
+      <c r="B34" s="24">
         <v>225</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="D34" s="20">
+      <c r="D34" s="19">
         <v>107</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="15" t="s">
         <v>2</v>
       </c>
       <c r="F34" s="3" t="s">
@@ -1967,49 +1980,49 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B35" s="24">
+      <c r="B35" s="23">
         <v>200</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="24">
+      <c r="D35" s="23">
         <v>115</v>
       </c>
-      <c r="E35" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F35" s="23" t="s">
+      <c r="E35" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="G35" s="23" t="s">
+      <c r="G35" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="H35" s="23" t="s">
+      <c r="H35" s="22" t="s">
         <v>54</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="B36" s="20">
+      <c r="B36" s="19">
         <v>300</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="20">
+      <c r="D36" s="19">
         <v>138</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E36" s="15" t="s">
         <v>2</v>
       </c>
       <c r="F36" s="3" t="s">
@@ -2023,17 +2036,17 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B37" s="17">
+      <c r="B37" s="16">
         <v>213700</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="C37" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="16">
         <v>103</v>
       </c>
       <c r="E37" s="1" t="s">
@@ -2050,17 +2063,17 @@
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B38" s="17">
+      <c r="B38" s="16">
         <v>259500</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="16">
         <v>104</v>
       </c>
       <c r="E38" s="1" t="s">
@@ -2077,17 +2090,17 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B39" s="17">
+      <c r="B39" s="16">
         <v>225</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="16">
         <v>115</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -2104,17 +2117,17 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B40" s="17">
+      <c r="B40" s="16">
         <v>250</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D40" s="16">
         <v>130</v>
       </c>
       <c r="E40" s="1" t="s">
@@ -2131,17 +2144,17 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="17">
+      <c r="B41" s="16">
         <v>185</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D41" s="16">
         <v>126</v>
       </c>
       <c r="E41" s="1" t="s">
@@ -2161,45 +2174,45 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="22" t="s">
         <v>142</v>
       </c>
       <c r="B42" s="23">
         <v>192500</v>
       </c>
-      <c r="C42" s="23" t="s">
+      <c r="C42" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="D42" s="23">
+      <c r="D42" s="22">
         <v>77</v>
       </c>
-      <c r="E42" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F42" s="23" t="s">
+      <c r="E42" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="23" t="s">
+      <c r="G42" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="H42" s="23" t="s">
+      <c r="H42" s="22" t="s">
         <v>54</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B43" s="17">
+      <c r="B43" s="16">
         <v>22500</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="16">
         <v>120</v>
       </c>
       <c r="E43" s="1" t="s">
@@ -2214,17 +2227,17 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B44" s="17">
+      <c r="B44" s="16">
         <v>225</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="17">
+      <c r="D44" s="16">
         <v>103</v>
       </c>
       <c r="E44" s="1" t="s">
@@ -2242,43 +2255,45 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="B45" s="17">
+      <c r="B45" s="33">
         <v>245</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="D45" s="17">
+      <c r="D45" s="33">
         <v>120</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F45" s="1" t="s">
+      <c r="E45" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="G45" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="H45" s="1"/>
+      <c r="H45" s="32" t="s">
+        <v>179</v>
+      </c>
       <c r="I45" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="28" t="s">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="B46" s="17">
+      <c r="B46" s="16">
         <v>275</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="D46" s="17">
+      <c r="D46" s="16">
         <v>137</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -2295,7 +2310,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>175</v>
       </c>
@@ -2324,9 +2339,9 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -2335,9 +2350,9 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2346,9 +2361,9 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -2357,9 +2372,9 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -2368,9 +2383,9 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -2379,9 +2394,9 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -2390,9 +2405,9 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -2401,9 +2416,9 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -2412,9 +2427,9 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -2423,9 +2438,9 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -2434,9 +2449,9 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -2445,9 +2460,9 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -2456,9 +2471,9 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -2467,9 +2482,9 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -2478,9 +2493,9 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -2489,9 +2504,9 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -2500,9 +2515,9 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -2511,9 +2526,9 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -2522,9 +2537,9 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -2533,9 +2548,9 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -2544,9 +2559,9 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -2555,9 +2570,9 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -2566,9 +2581,9 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="17"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -2577,9 +2592,9 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -2588,9 +2603,9 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -2599,9 +2614,9 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -2610,9 +2625,9 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="17"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -2621,9 +2636,9 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="17"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="16"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
@@ -2632,9 +2647,9 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -2643,9 +2658,9 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="16"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -2654,9 +2669,9 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="17"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -2665,9 +2680,9 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="17"/>
-      <c r="D79" s="17"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="16"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -2676,9 +2691,9 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="17"/>
-      <c r="D80" s="17"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
@@ -2687,9 +2702,9 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
-      <c r="B81" s="17"/>
-      <c r="C81" s="17"/>
-      <c r="D81" s="17"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -2698,9 +2713,9 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
-      <c r="B82" s="17"/>
-      <c r="C82" s="17"/>
-      <c r="D82" s="17"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="16"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
@@ -2709,9 +2724,9 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
-      <c r="B83" s="17"/>
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
+      <c r="B83" s="16"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="16"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
@@ -2720,9 +2735,9 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
-      <c r="B84" s="17"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="16"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
@@ -2731,9 +2746,9 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="17"/>
-      <c r="D85" s="17"/>
+      <c r="B85" s="16"/>
+      <c r="C85" s="16"/>
+      <c r="D85" s="16"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
@@ -2742,9 +2757,9 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
-      <c r="B86" s="17"/>
-      <c r="C86" s="17"/>
-      <c r="D86" s="17"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="16"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
@@ -2753,9 +2768,9 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
-      <c r="B87" s="17"/>
-      <c r="C87" s="17"/>
-      <c r="D87" s="17"/>
+      <c r="B87" s="16"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="16"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
@@ -2764,9 +2779,9 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
-      <c r="B88" s="17"/>
-      <c r="C88" s="17"/>
-      <c r="D88" s="17"/>
+      <c r="B88" s="16"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="16"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
@@ -2775,9 +2790,9 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="17"/>
-      <c r="D89" s="17"/>
+      <c r="B89" s="16"/>
+      <c r="C89" s="16"/>
+      <c r="D89" s="16"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
@@ -2786,9 +2801,9 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
-      <c r="B90" s="17"/>
-      <c r="C90" s="17"/>
-      <c r="D90" s="17"/>
+      <c r="B90" s="16"/>
+      <c r="C90" s="16"/>
+      <c r="D90" s="16"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
@@ -2797,9 +2812,9 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
-      <c r="B91" s="17"/>
-      <c r="C91" s="17"/>
-      <c r="D91" s="17"/>
+      <c r="B91" s="16"/>
+      <c r="C91" s="16"/>
+      <c r="D91" s="16"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
@@ -2808,9 +2823,9 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
-      <c r="B92" s="17"/>
-      <c r="C92" s="17"/>
-      <c r="D92" s="17"/>
+      <c r="B92" s="16"/>
+      <c r="C92" s="16"/>
+      <c r="D92" s="16"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
@@ -2818,6 +2833,21 @@
       <c r="I92" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A3:I47">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="YES"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <filters>
+        <filter val="22 June 16:15"/>
+        <filter val="22 June 8:50am"/>
+        <filter val="22 Juni 2018 11AM"/>
+        <filter val="22 juni 2018 om 2:30 uur"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="I9" r:id="rId1"/>
     <hyperlink ref="I5" r:id="rId2"/>
@@ -2859,7 +2889,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the views for saturday
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="181">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -596,6 +596,9 @@
   </si>
   <si>
     <t>See, Thinking</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -713,16 +716,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1099,19 +1099,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="15" style="20" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="20" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="15" style="19" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="19" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" customWidth="1"/>
     <col min="7" max="7" width="37" bestFit="1" customWidth="1"/>
@@ -1120,27 +1119,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="12" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="12"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>95</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1159,13 +1158,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1182,20 +1181,20 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>200</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -1209,71 +1208,71 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>200</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="22" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="22">
         <v>225</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="22">
         <v>88</v>
       </c>
-      <c r="E7" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="22" t="s">
+      <c r="E7" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="21" t="s">
         <v>54</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>200</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1286,15 +1285,15 @@
       <c r="H8" s="3"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>200</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1309,15 +1308,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>215</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1328,19 +1327,19 @@
         <v>1</v>
       </c>
       <c r="H10" s="3"/>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>200</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="2" t="s">
         <v>2</v>
       </c>
@@ -1355,17 +1354,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="15">
         <v>225</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="15">
         <v>109</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1383,70 +1382,70 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="22">
         <v>210</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="21">
         <v>106</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="22" t="s">
+      <c r="E13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="I13" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="13">
         <v>190</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="15" t="s">
+      <c r="D14" s="18"/>
+      <c r="E14" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>86</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>200</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="2" t="s">
         <v>2</v>
       </c>
@@ -1461,17 +1460,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>200</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="6"/>
       <c r="E16" s="2" t="s">
         <v>2</v>
       </c>
@@ -1482,82 +1481,82 @@
         <v>1</v>
       </c>
       <c r="H16" s="3"/>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17" s="22">
         <v>225</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="21">
         <v>122</v>
       </c>
-      <c r="E17" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="22" t="s">
+      <c r="E17" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="G17" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="21" t="s">
         <v>54</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+    <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B18" s="29">
         <v>229500</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="22">
         <v>115</v>
       </c>
-      <c r="E18" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="22" t="s">
+      <c r="E18" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="21" t="s">
         <v>54</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+    <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B19" s="23">
         <v>210</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="24">
         <v>106</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="12" t="s">
         <v>2</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -1566,24 +1565,24 @@
       <c r="G19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="12" t="s">
         <v>110</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>199500</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="2" t="s">
         <v>2</v>
       </c>
@@ -1593,22 +1592,22 @@
       <c r="G20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="10"/>
+      <c r="H20" s="9"/>
       <c r="I20" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>200</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="7"/>
+      <c r="D21" s="6"/>
       <c r="E21" s="2" t="s">
         <v>2</v>
       </c>
@@ -1623,46 +1622,46 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+    <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B22" s="29">
         <v>200</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="22">
         <v>111</v>
       </c>
-      <c r="E22" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22" s="22" t="s">
+      <c r="E22" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="22" t="s">
+      <c r="G22" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="H22" s="22" t="s">
+      <c r="H22" s="21" t="s">
         <v>145</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <v>225</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="7"/>
+      <c r="D23" s="6"/>
       <c r="E23" s="2" t="s">
         <v>2</v>
       </c>
@@ -1677,46 +1676,46 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
+    <row r="24" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A24" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="22">
         <v>235</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="22">
         <v>111</v>
       </c>
-      <c r="E24" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" s="22" t="s">
+      <c r="E24" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="H24" s="22" t="s">
+      <c r="H24" s="21" t="s">
         <v>54</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="15">
         <v>225</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="15">
         <v>115</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -1733,17 +1732,17 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="16">
+      <c r="B26" s="15">
         <v>219500</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="16"/>
+      <c r="D26" s="15"/>
       <c r="E26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1754,21 +1753,21 @@
         <v>84</v>
       </c>
       <c r="H26" s="1"/>
-      <c r="I26" s="10" t="s">
+      <c r="I26" s="9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <v>225</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>123</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -1781,50 +1780,50 @@
         <v>1</v>
       </c>
       <c r="H27" s="1"/>
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+    <row r="28" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="23">
+      <c r="B28" s="22">
         <v>215</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="22">
         <v>105</v>
       </c>
-      <c r="E28" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F28" s="22" t="s">
+      <c r="E28" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="H28" s="22" t="s">
+      <c r="H28" s="21" t="s">
         <v>54</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B29" s="28">
+      <c r="B29" s="27">
         <v>260</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="28">
+      <c r="D29" s="27">
         <v>148</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -1841,105 +1840,107 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="30">
+      <c r="B30" s="29">
         <v>225</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="23">
+      <c r="D30" s="22">
         <v>124</v>
       </c>
-      <c r="E30" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F30" s="22" t="s">
+      <c r="E30" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="22" t="s">
+      <c r="G30" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="H30" s="22" t="s">
+      <c r="H30" s="21" t="s">
         <v>174</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="29">
         <v>179</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="16">
+      <c r="D31" s="22">
         <v>99</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F31" s="1" t="s">
+      <c r="E31" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="H31" s="1"/>
+      <c r="H31" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="I31" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="B32" s="23">
+      <c r="B32" s="22">
         <v>195</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="23">
+      <c r="D32" s="22">
         <v>80</v>
       </c>
-      <c r="E32" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F32" s="22" t="s">
+      <c r="E32" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="G32" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="H32" s="22" t="s">
+      <c r="H32" s="21" t="s">
         <v>54</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B33" s="24">
+      <c r="B33" s="23">
         <v>225</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="D33" s="19">
+      <c r="D33" s="18">
         <v>107</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="14" t="s">
         <v>2</v>
       </c>
       <c r="F33" s="3" t="s">
@@ -1953,20 +1954,20 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="B34" s="24">
+      <c r="B34" s="23">
         <v>225</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C34" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D34" s="19">
+      <c r="D34" s="18">
         <v>107</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="14" t="s">
         <v>2</v>
       </c>
       <c r="F34" s="3" t="s">
@@ -1980,49 +1981,49 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="B35" s="23">
+      <c r="B35" s="22">
         <v>200</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D35" s="22">
         <v>115</v>
       </c>
-      <c r="E35" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F35" s="22" t="s">
+      <c r="E35" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G35" s="22" t="s">
+      <c r="G35" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="H35" s="22" t="s">
+      <c r="H35" s="21" t="s">
         <v>54</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="29" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="B36" s="19">
+      <c r="B36" s="18">
         <v>300</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="19">
+      <c r="D36" s="18">
         <v>138</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="14" t="s">
         <v>2</v>
       </c>
       <c r="F36" s="3" t="s">
@@ -2036,17 +2037,17 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B37" s="16">
+      <c r="B37" s="15">
         <v>213700</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="D37" s="16">
+      <c r="D37" s="15">
         <v>103</v>
       </c>
       <c r="E37" s="1" t="s">
@@ -2063,17 +2064,17 @@
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B38" s="16">
+      <c r="B38" s="15">
         <v>259500</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="15">
         <v>104</v>
       </c>
       <c r="E38" s="1" t="s">
@@ -2090,17 +2091,17 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B39" s="16">
+      <c r="B39" s="15">
         <v>225</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="15">
         <v>115</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -2117,17 +2118,17 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B40" s="16">
+      <c r="B40" s="15">
         <v>250</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="D40" s="16">
+      <c r="D40" s="15">
         <v>130</v>
       </c>
       <c r="E40" s="1" t="s">
@@ -2144,29 +2145,29 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="16">
+      <c r="B41" s="22">
         <v>185</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="D41" s="16">
+      <c r="D41" s="22">
         <v>126</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F41" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G41" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H41" s="21" t="s">
         <v>89</v>
       </c>
       <c r="I41" s="5" t="s">
@@ -2174,45 +2175,45 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="B42" s="23">
+      <c r="B42" s="22">
         <v>192500</v>
       </c>
-      <c r="C42" s="22" t="s">
+      <c r="C42" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="D42" s="22">
+      <c r="D42" s="21">
         <v>77</v>
       </c>
-      <c r="E42" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F42" s="22" t="s">
+      <c r="E42" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="22" t="s">
+      <c r="G42" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="H42" s="22" t="s">
+      <c r="H42" s="21" t="s">
         <v>54</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B43" s="16">
+      <c r="B43" s="15">
         <v>22500</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="D43" s="16">
+      <c r="D43" s="15">
         <v>120</v>
       </c>
       <c r="E43" s="1" t="s">
@@ -2227,73 +2228,75 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="B44" s="16">
+      <c r="B44" s="31">
         <v>225</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="16">
+      <c r="D44" s="31">
         <v>103</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F44" s="1" t="s">
+      <c r="E44" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G44" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1" t="s">
+      <c r="H44" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="I44" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="B45" s="33">
+      <c r="B45" s="32">
         <v>245</v>
       </c>
-      <c r="C45" s="33" t="s">
+      <c r="C45" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="D45" s="33">
+      <c r="D45" s="32">
         <v>120</v>
       </c>
-      <c r="E45" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F45" s="32" t="s">
+      <c r="E45" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="G45" s="32" t="s">
+      <c r="G45" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="H45" s="32" t="s">
+      <c r="H45" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="I45" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="27" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="B46" s="16">
+      <c r="B46" s="15">
         <v>275</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="C46" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="D46" s="16">
+      <c r="D46" s="15">
         <v>137</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -2310,7 +2313,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>175</v>
       </c>
@@ -2339,9 +2342,9 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -2350,9 +2353,9 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2361,9 +2364,9 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -2372,20 +2375,22 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
+      <c r="I51" s="1" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -2394,9 +2399,9 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -2405,9 +2410,9 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -2416,9 +2421,9 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -2427,9 +2432,9 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -2438,9 +2443,9 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -2449,9 +2454,9 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -2460,9 +2465,9 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -2471,9 +2476,9 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -2482,9 +2487,9 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -2493,9 +2498,9 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -2504,9 +2509,9 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -2515,9 +2520,9 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -2526,9 +2531,9 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -2537,9 +2542,9 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-      <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -2548,9 +2553,9 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-      <c r="B67" s="16"/>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -2559,9 +2564,9 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="16"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -2570,9 +2575,9 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="16"/>
-      <c r="D69" s="16"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -2581,9 +2586,9 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="16"/>
+      <c r="B70" s="15"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -2592,9 +2597,9 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="16"/>
-      <c r="D71" s="16"/>
+      <c r="B71" s="15"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -2603,9 +2608,9 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
-      <c r="B72" s="16"/>
-      <c r="C72" s="16"/>
-      <c r="D72" s="16"/>
+      <c r="B72" s="15"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -2614,9 +2619,9 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
-      <c r="B73" s="16"/>
-      <c r="C73" s="16"/>
-      <c r="D73" s="16"/>
+      <c r="B73" s="15"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -2625,9 +2630,9 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
-      <c r="D74" s="16"/>
+      <c r="B74" s="15"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -2636,9 +2641,9 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
-      <c r="B75" s="16"/>
-      <c r="C75" s="16"/>
-      <c r="D75" s="16"/>
+      <c r="B75" s="15"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
@@ -2647,9 +2652,9 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
-      <c r="B76" s="16"/>
-      <c r="C76" s="16"/>
-      <c r="D76" s="16"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -2658,9 +2663,9 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
-      <c r="B77" s="16"/>
-      <c r="C77" s="16"/>
-      <c r="D77" s="16"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -2669,9 +2674,9 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
-      <c r="B78" s="16"/>
-      <c r="C78" s="16"/>
-      <c r="D78" s="16"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -2680,9 +2685,9 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
-      <c r="B79" s="16"/>
-      <c r="C79" s="16"/>
-      <c r="D79" s="16"/>
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -2691,9 +2696,9 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
-      <c r="B80" s="16"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="16"/>
+      <c r="B80" s="15"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
@@ -2702,9 +2707,9 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
-      <c r="B81" s="16"/>
-      <c r="C81" s="16"/>
-      <c r="D81" s="16"/>
+      <c r="B81" s="15"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="15"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -2713,9 +2718,9 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
-      <c r="B82" s="16"/>
-      <c r="C82" s="16"/>
-      <c r="D82" s="16"/>
+      <c r="B82" s="15"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="15"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
@@ -2724,9 +2729,9 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
-      <c r="B83" s="16"/>
-      <c r="C83" s="16"/>
-      <c r="D83" s="16"/>
+      <c r="B83" s="15"/>
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
@@ -2735,9 +2740,9 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
-      <c r="B84" s="16"/>
-      <c r="C84" s="16"/>
-      <c r="D84" s="16"/>
+      <c r="B84" s="15"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="15"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
@@ -2746,9 +2751,9 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
-      <c r="B85" s="16"/>
-      <c r="C85" s="16"/>
-      <c r="D85" s="16"/>
+      <c r="B85" s="15"/>
+      <c r="C85" s="15"/>
+      <c r="D85" s="15"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
@@ -2757,9 +2762,9 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
-      <c r="B86" s="16"/>
-      <c r="C86" s="16"/>
-      <c r="D86" s="16"/>
+      <c r="B86" s="15"/>
+      <c r="C86" s="15"/>
+      <c r="D86" s="15"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
@@ -2768,9 +2773,9 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
-      <c r="B87" s="16"/>
-      <c r="C87" s="16"/>
-      <c r="D87" s="16"/>
+      <c r="B87" s="15"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="15"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
@@ -2779,9 +2784,9 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
-      <c r="B88" s="16"/>
-      <c r="C88" s="16"/>
-      <c r="D88" s="16"/>
+      <c r="B88" s="15"/>
+      <c r="C88" s="15"/>
+      <c r="D88" s="15"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
@@ -2790,9 +2795,9 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
-      <c r="B89" s="16"/>
-      <c r="C89" s="16"/>
-      <c r="D89" s="16"/>
+      <c r="B89" s="15"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
@@ -2801,9 +2806,9 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
-      <c r="B90" s="16"/>
-      <c r="C90" s="16"/>
-      <c r="D90" s="16"/>
+      <c r="B90" s="15"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="15"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
@@ -2812,9 +2817,9 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
-      <c r="B91" s="16"/>
-      <c r="C91" s="16"/>
-      <c r="D91" s="16"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="15"/>
+      <c r="D91" s="15"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
@@ -2823,9 +2828,9 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
-      <c r="B92" s="16"/>
-      <c r="C92" s="16"/>
-      <c r="D92" s="16"/>
+      <c r="B92" s="15"/>
+      <c r="C92" s="15"/>
+      <c r="D92" s="15"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
@@ -2833,21 +2838,6 @@
       <c r="I92" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:I47">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="YES"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <filters>
-        <filter val="22 June 16:15"/>
-        <filter val="22 June 8:50am"/>
-        <filter val="22 Juni 2018 11AM"/>
-        <filter val="22 juni 2018 om 2:30 uur"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <hyperlinks>
     <hyperlink ref="I9" r:id="rId1"/>
     <hyperlink ref="I5" r:id="rId2"/>
@@ -2872,9 +2862,11 @@
     <hyperlink ref="I42" r:id="rId21"/>
     <hyperlink ref="I33" r:id="rId22"/>
     <hyperlink ref="I38" r:id="rId23"/>
+    <hyperlink ref="I45" r:id="rId24"/>
+    <hyperlink ref="I44" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
 
@@ -2889,7 +2881,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Willem Pijperstraat 41
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Karnan\funda\fundanl\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4095" tabRatio="309"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14388" windowHeight="4092" tabRatio="309"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="188">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -608,12 +613,24 @@
   </si>
   <si>
     <t>Bidding sent for 250000</t>
+  </si>
+  <si>
+    <t>Willem Pijperstraat 41</t>
+  </si>
+  <si>
+    <t>1323 TG Almere</t>
+  </si>
+  <si>
+    <t>04-July-2018 5PM</t>
+  </si>
+  <si>
+    <t>https://www.funda.nl/koop/almere/huis-40627928-willem-pijperstraat-41/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1096,7 +1113,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1106,24 +1123,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B7" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:I49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="19" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" style="19" customWidth="1"/>
     <col min="3" max="3" width="15" style="19" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="19" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" customWidth="1"/>
     <col min="7" max="7" width="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="75.85546875" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="75.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" s="20" t="s">
         <v>34</v>
       </c>
@@ -1163,7 +1180,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1186,7 +1203,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>3</v>
       </c>
@@ -1213,7 +1230,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>4</v>
       </c>
@@ -1240,7 +1257,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>5</v>
       </c>
@@ -1269,7 +1286,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1290,7 +1307,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1313,7 +1330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1336,7 +1353,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1359,7 +1376,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>24</v>
       </c>
@@ -1388,7 +1405,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>25</v>
       </c>
@@ -1417,7 +1434,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>29</v>
       </c>
@@ -1442,7 +1459,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1467,7 +1484,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -1492,7 +1509,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>43</v>
       </c>
@@ -1521,7 +1538,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>45</v>
       </c>
@@ -1550,7 +1567,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>49</v>
       </c>
@@ -1579,7 +1596,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>56</v>
       </c>
@@ -1604,7 +1621,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>59</v>
       </c>
@@ -1629,7 +1646,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
         <v>62</v>
       </c>
@@ -1658,7 +1675,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>65</v>
       </c>
@@ -1683,7 +1700,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
         <v>68</v>
       </c>
@@ -1712,7 +1729,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
@@ -1739,7 +1756,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
@@ -1764,7 +1781,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>90</v>
       </c>
@@ -1820,7 +1837,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>97</v>
       </c>
@@ -1847,7 +1864,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="28" t="s">
         <v>100</v>
       </c>
@@ -1876,7 +1893,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
         <v>103</v>
       </c>
@@ -1905,7 +1922,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
         <v>106</v>
       </c>
@@ -1934,7 +1951,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>112</v>
       </c>
@@ -1961,7 +1978,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>115</v>
       </c>
@@ -1988,7 +2005,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>118</v>
       </c>
@@ -2017,7 +2034,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
         <v>120</v>
       </c>
@@ -2044,7 +2061,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>123</v>
       </c>
@@ -2073,7 +2090,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>126</v>
       </c>
@@ -2100,7 +2117,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>129</v>
       </c>
@@ -2127,7 +2144,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>132</v>
       </c>
@@ -2154,7 +2171,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="21" t="s">
         <v>135</v>
       </c>
@@ -2183,7 +2200,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="21" t="s">
         <v>142</v>
       </c>
@@ -2212,7 +2229,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>146</v>
       </c>
@@ -2237,7 +2254,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="29" t="s">
         <v>160</v>
       </c>
@@ -2266,7 +2283,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="21" t="s">
         <v>163</v>
       </c>
@@ -2295,7 +2312,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="29" t="s">
         <v>168</v>
       </c>
@@ -2324,7 +2341,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>175</v>
       </c>
@@ -2351,7 +2368,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
         <v>180</v>
       </c>
@@ -2378,18 +2395,34 @@
         <v>134</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B49" s="1">
+        <v>250</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D49" s="1">
+        <v>124</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="I49" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
@@ -2400,7 +2433,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
@@ -2413,7 +2446,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
@@ -2424,7 +2457,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
@@ -2435,7 +2468,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
@@ -2446,7 +2479,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
@@ -2457,7 +2490,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
@@ -2468,7 +2501,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
@@ -2479,7 +2512,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
@@ -2490,7 +2523,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
@@ -2501,7 +2534,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
@@ -2512,7 +2545,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
@@ -2523,7 +2556,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="15"/>
       <c r="C62" s="15"/>
@@ -2534,7 +2567,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="15"/>
       <c r="C63" s="15"/>
@@ -2545,7 +2578,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
@@ -2556,7 +2589,7 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
@@ -2567,7 +2600,7 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
@@ -2578,7 +2611,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
@@ -2589,7 +2622,7 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
@@ -2600,7 +2633,7 @@
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="15"/>
       <c r="C69" s="15"/>
@@ -2611,7 +2644,7 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="15"/>
       <c r="C70" s="15"/>
@@ -2622,7 +2655,7 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
@@ -2633,7 +2666,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="15"/>
       <c r="C72" s="15"/>
@@ -2644,7 +2677,7 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="15"/>
       <c r="C73" s="15"/>
@@ -2655,7 +2688,7 @@
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="15"/>
       <c r="C74" s="15"/>
@@ -2666,7 +2699,7 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="15"/>
       <c r="C75" s="15"/>
@@ -2677,7 +2710,7 @@
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="15"/>
       <c r="C76" s="15"/>
@@ -2688,7 +2721,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="15"/>
       <c r="C77" s="15"/>
@@ -2699,7 +2732,7 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="15"/>
       <c r="C78" s="15"/>
@@ -2710,7 +2743,7 @@
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="15"/>
       <c r="C79" s="15"/>
@@ -2721,7 +2754,7 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="15"/>
       <c r="C80" s="15"/>
@@ -2732,7 +2765,7 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="15"/>
       <c r="C81" s="15"/>
@@ -2743,7 +2776,7 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="15"/>
       <c r="C82" s="15"/>
@@ -2754,7 +2787,7 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="15"/>
       <c r="C83" s="15"/>
@@ -2765,7 +2798,7 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="15"/>
       <c r="C84" s="15"/>
@@ -2776,7 +2809,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="15"/>
       <c r="C85" s="15"/>
@@ -2787,7 +2820,7 @@
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="15"/>
       <c r="C86" s="15"/>
@@ -2798,7 +2831,7 @@
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="15"/>
       <c r="C87" s="15"/>
@@ -2809,7 +2842,7 @@
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="15"/>
       <c r="C88" s="15"/>
@@ -2820,7 +2853,7 @@
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="15"/>
       <c r="C89" s="15"/>
@@ -2831,7 +2864,7 @@
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="15"/>
       <c r="C90" s="15"/>
@@ -2842,7 +2875,7 @@
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="15"/>
       <c r="C91" s="15"/>
@@ -2853,7 +2886,7 @@
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="15"/>
       <c r="C92" s="15"/>
@@ -2905,7 +2938,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
@@ -2925,7 +2958,7 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Alban Bergstraat 18
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="194">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -600,9 +600,6 @@
     <t>03 July 4PM</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>Couperinstraat 23</t>
   </si>
   <si>
@@ -637,6 +634,15 @@
   </si>
   <si>
     <t>https://www.funda.nl/koop/almere/huis-40617611-contrabasweg-159/</t>
+  </si>
+  <si>
+    <t>Alban Bergstraat 18</t>
+  </si>
+  <si>
+    <t>1323 GH Almere</t>
+  </si>
+  <si>
+    <t>https://www.funda.nl/koop/almere/huis-40623916-alban-bergstraat-18/</t>
   </si>
 </sst>
 </file>
@@ -1135,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:I50"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1411,7 +1417,7 @@
         <v>172</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>23</v>
@@ -2289,7 +2295,7 @@
         <v>166</v>
       </c>
       <c r="H44" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I44" s="5" t="s">
         <v>162</v>
@@ -2347,7 +2353,7 @@
         <v>171</v>
       </c>
       <c r="H46" s="29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>170</v>
@@ -2382,7 +2388,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B48" s="18">
         <v>250</v>
@@ -2409,13 +2415,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B49" s="1">
         <v>250</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D49" s="1">
         <v>124</v>
@@ -2427,22 +2433,22 @@
         <v>76</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B50" s="1">
         <v>220</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D50" s="1">
         <v>112</v>
@@ -2454,24 +2460,36 @@
         <v>76</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+      <c r="B51" s="1">
+        <v>250</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D51" s="1">
+        <v>120</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Anna Bijnsstraat 4
</commit_message>
<xml_diff>
--- a/Funda.xlsx
+++ b/Funda.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="204">
   <si>
     <t>Basilicumweg 161 Almere</t>
   </si>
@@ -598,12 +598,6 @@
     <t>Couperinstraat 23</t>
   </si>
   <si>
-    <t>Bidding sent for 240100</t>
-  </si>
-  <si>
-    <t>Interested</t>
-  </si>
-  <si>
     <t>Bidding sent for 250000</t>
   </si>
   <si>
@@ -625,9 +619,6 @@
     <t>1311 LA Almere</t>
   </si>
   <si>
-    <t>09-July-2018 4PM</t>
-  </si>
-  <si>
     <t>https://www.funda.nl/koop/almere/huis-40617611-contrabasweg-159/</t>
   </si>
   <si>
@@ -650,6 +641,33 @@
   </si>
   <si>
     <t>https://www.funda.nl/koop/almere/huis-40635120-fagotstraat-12/</t>
+  </si>
+  <si>
+    <t>Alban Bergstraat 3</t>
+  </si>
+  <si>
+    <t>18-July-2018 4PM</t>
+  </si>
+  <si>
+    <t>https://www.funda.nl/koop/almere/huis-40623916-alban-bergstraat-3/</t>
+  </si>
+  <si>
+    <t>Lost Bidding</t>
+  </si>
+  <si>
+    <t>Onhold</t>
+  </si>
+  <si>
+    <t>Waiting for result</t>
+  </si>
+  <si>
+    <t>Anna Bijnsstraat 4</t>
+  </si>
+  <si>
+    <t>1321 VP Almere</t>
+  </si>
+  <si>
+    <t>https://www.funda.nl/koop/almere/huis-40716599-anna-bijnsstraat-4/</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1156,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1148,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D37" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B38" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,7 +1426,7 @@
       <c r="B12" s="30">
         <v>225</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="30" t="s">
         <v>173</v>
       </c>
       <c r="D12" s="30">
@@ -1424,7 +1442,7 @@
         <v>172</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>23</v>
@@ -1437,7 +1455,7 @@
       <c r="B13" s="22">
         <v>210</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="22" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="22">
@@ -1541,7 +1559,7 @@
       <c r="B17" s="22">
         <v>225</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="22" t="s">
         <v>44</v>
       </c>
       <c r="D17" s="22">
@@ -2232,7 +2250,7 @@
       <c r="B42" s="22">
         <v>192500</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="C42" s="22" t="s">
         <v>143</v>
       </c>
       <c r="D42" s="22">
@@ -2286,7 +2304,7 @@
       <c r="B44" s="30">
         <v>225</v>
       </c>
-      <c r="C44" s="29" t="s">
+      <c r="C44" s="30" t="s">
         <v>161</v>
       </c>
       <c r="D44" s="30">
@@ -2302,7 +2320,7 @@
         <v>166</v>
       </c>
       <c r="H44" s="29" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="I44" s="5" t="s">
         <v>162</v>
@@ -2315,7 +2333,7 @@
       <c r="B45" s="22">
         <v>245</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="C45" s="22" t="s">
         <v>164</v>
       </c>
       <c r="D45" s="22">
@@ -2344,7 +2362,7 @@
       <c r="B46" s="30">
         <v>275</v>
       </c>
-      <c r="C46" s="29" t="s">
+      <c r="C46" s="30" t="s">
         <v>169</v>
       </c>
       <c r="D46" s="30">
@@ -2360,35 +2378,37 @@
         <v>171</v>
       </c>
       <c r="H46" s="29" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="22">
         <v>235</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="D47" s="15">
+      <c r="D47" s="22">
         <v>114</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F47" s="1" t="s">
+      <c r="E47" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G47" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="H47" s="1"/>
+      <c r="H47" s="21" t="s">
+        <v>145</v>
+      </c>
       <c r="I47" s="1" t="s">
         <v>176</v>
       </c>
@@ -2400,7 +2420,7 @@
       <c r="B48" s="18">
         <v>250</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="18" t="s">
         <v>133</v>
       </c>
       <c r="D48" s="18">
@@ -2422,13 +2442,13 @@
     </row>
     <row r="49" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B49" s="15">
         <v>250</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>184</v>
+      <c r="C49" s="15" t="s">
+        <v>182</v>
       </c>
       <c r="D49" s="15">
         <v>124</v>
@@ -2440,49 +2460,51 @@
         <v>76</v>
       </c>
       <c r="G49" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1" t="s">
+      <c r="B50" s="18">
+        <v>220</v>
+      </c>
+      <c r="C50" s="18" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="D50" s="18">
+        <v>112</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H50" s="14"/>
+      <c r="I50" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="B50" s="15">
-        <v>220</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D50" s="15">
-        <v>112</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B51" s="15">
         <v>250</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>192</v>
+      <c r="C51" s="15" t="s">
+        <v>189</v>
       </c>
       <c r="D51" s="15">
         <v>120</v>
@@ -2494,61 +2516,95 @@
         <v>47</v>
       </c>
       <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
+      <c r="H51" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="I51" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="B52" s="22">
+        <v>239500</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="D52" s="22">
+        <v>110</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G52" s="21" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="H52" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="I52" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="B52" s="15">
-        <v>239500</v>
-      </c>
-      <c r="C52" s="1" t="s">
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D52" s="15">
-        <v>110</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F52" s="1" t="s">
+      <c r="B53" s="15">
+        <v>250</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="D53" s="15">
+        <v>108</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1" t="s">
+      <c r="H53" s="1"/>
+      <c r="I53" s="5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-    </row>
-    <row r="54" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B54" s="15">
+        <v>250</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D54" s="15">
+        <v>109</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-    </row>
-    <row r="55" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="I54" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
@@ -2647,7 +2703,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
@@ -2658,7 +2714,7 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
@@ -2669,7 +2725,7 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
@@ -2993,9 +3049,10 @@
     <hyperlink ref="I38" r:id="rId23"/>
     <hyperlink ref="I45" r:id="rId24"/>
     <hyperlink ref="I44" r:id="rId25"/>
+    <hyperlink ref="I53" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
 

</xml_diff>